<commit_message>
Adding references to example sheets.
</commit_message>
<xml_diff>
--- a/ExcelExamples/ZARSwap.xlsx
+++ b/ExcelExamples/ZARSwap.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="10290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateSwap" sheetId="1" r:id="rId1"/>
     <sheet name="ViewSwap" sheetId="2" r:id="rId2"/>
     <sheet name="ValueSwap" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcMode="manual" calcOnSave="0"/>
+  <calcPr calcId="145621" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>QSA.ValueZARSwap</t>
+  </si>
+  <si>
+    <t>QSA.GetAvailableResults</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +115,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,7 +179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -185,6 +195,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,10 +608,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F27"/>
+  <dimension ref="B2:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,14 +621,18 @@
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I2" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -625,8 +640,12 @@
         <f>_xll.QSA.GetResults(CreateSwap!$B$10,B3)</f>
         <v>8.1199999999999994E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I3" s="7" t="str">
+        <f t="array" aca="1" ref="I3:I10" ca="1">_xll.QSA.GetAvailableResults(CreateSwap!B10)</f>
+        <v>accrualFractions</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>11</v>
       </c>
@@ -634,8 +653,12 @@
         <f>_xll.QSA.GetResults(CreateSwap!$B$10,B4)</f>
         <v>ZAR:JIBAR:3M</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="7" t="str">
+        <f ca="1"/>
+        <v>fixedRate</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
@@ -643,8 +666,18 @@
         <f>_xll.QSA.GetResults(CreateSwap!$B$10,B5)</f>
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="str">
+        <f ca="1"/>
+        <v>index</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="7" t="str">
+        <f ca="1"/>
+        <v>indexDates</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
@@ -660,8 +693,12 @@
       <c r="F7" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I7" s="7" t="str">
+        <f ca="1"/>
+        <v>notionals</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <f t="array" ref="B8:B27">_xll.QSA.GetResults(CreateSwap!$B$10,B7)</f>
         <v>1000000</v>
@@ -682,8 +719,12 @@
         <f t="array" ref="F8:F27">_xll.QSA.GetResults(CreateSwap!$B$10,F7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I8" s="7" t="str">
+        <f ca="1"/>
+        <v>payDates</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>1000000</v>
       </c>
@@ -699,8 +740,12 @@
       <c r="F9" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I9" s="7" t="str">
+        <f ca="1"/>
+        <v>payFixed</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>1000000</v>
       </c>
@@ -716,8 +761,12 @@
       <c r="F10" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I10" s="7" t="str">
+        <f ca="1"/>
+        <v>spreads</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>1000000</v>
       </c>
@@ -734,7 +783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>1000000</v>
       </c>
@@ -751,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>1000000</v>
       </c>
@@ -768,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>1000000</v>
       </c>
@@ -785,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>1000000</v>
       </c>
@@ -802,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>1000000</v>
       </c>
@@ -1008,6 +1057,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>